<commit_message>
Update resume and CV
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelsieler/Dropbox/Mac (2)/Documents/Project_Repos/curriculum-vitae/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5F1457D-FF08-664B-B753-70482F15AB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C1CE33-0ED4-9F49-AD10-D71B95824B3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -422,9 +422,6 @@
     <t>Multivariate linear regression</t>
   </si>
   <si>
-    <t>*estimated 2025*</t>
-  </si>
-  <si>
     <t>Oregon State University</t>
   </si>
   <si>
@@ -744,6 +741,9 @@
   </si>
   <si>
     <t>https://michaelsieler.com/en/latest/Projects/projects.html</t>
+  </si>
+  <si>
+    <t>estimated 2025 *</t>
   </si>
 </sst>
 </file>
@@ -1223,10 +1223,10 @@
     </row>
     <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -1238,25 +1238,25 @@
         <v>2023</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="H2" s="7" t="s">
         <v>203</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" t="s">
         <v>200</v>
-      </c>
-      <c r="C3" t="s">
-        <v>201</v>
       </c>
       <c r="D3">
         <v>2020</v>
@@ -1265,13 +1265,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
   </sheetData>
@@ -1324,22 +1324,22 @@
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D2">
         <v>2021</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G2" s="4"/>
     </row>
@@ -1391,42 +1391,42 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D2">
         <v>2022</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D3">
         <v>2021</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1477,13 +1477,13 @@
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D2">
         <v>2019</v>
@@ -1491,10 +1491,10 @@
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -1518,7 +1518,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49497E0-D611-F748-9047-7F39E42561EA}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1530,18 +1530,18 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -1583,13 +1583,13 @@
     </row>
     <row r="2" spans="1:4" ht="224" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1597,13 +1597,13 @@
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1617,7 +1617,7 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1631,7 +1631,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1645,7 +1645,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1694,7 +1694,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B2" t="s">
         <v>101</v>
@@ -1702,7 +1702,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1710,7 +1710,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B4" t="s">
         <v>85</v>
@@ -1718,7 +1718,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s">
         <v>102</v>
@@ -1726,7 +1726,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B6" t="s">
         <v>83</v>
@@ -1734,7 +1734,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>86</v>
@@ -1742,7 +1742,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
@@ -1750,7 +1750,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -1758,7 +1758,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B10" t="s">
         <v>84</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" t="s">
         <v>103</v>
@@ -1774,7 +1774,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B12" t="s">
         <v>100</v>
@@ -1782,15 +1782,15 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" t="s">
         <v>152</v>
-      </c>
-      <c r="B13" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>125</v>
@@ -1798,7 +1798,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>123</v>
@@ -1806,7 +1806,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>124</v>
@@ -1814,7 +1814,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B17" t="s">
         <v>116</v>
@@ -1822,7 +1822,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" t="s">
         <v>119</v>
@@ -1830,7 +1830,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>118</v>
@@ -1838,7 +1838,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B20" t="s">
         <v>117</v>
@@ -1846,7 +1846,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B21" t="s">
         <v>120</v>
@@ -1854,7 +1854,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>121</v>
@@ -1862,7 +1862,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
         <v>122</v>
@@ -1870,7 +1870,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" t="s">
         <v>111</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B25" t="s">
         <v>112</v>
@@ -1886,7 +1886,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" t="s">
         <v>113</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B27" t="s">
         <v>114</v>
@@ -1902,7 +1902,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B28" t="s">
         <v>115</v>
@@ -1910,7 +1910,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
         <v>106</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
         <v>107</v>
@@ -1926,7 +1926,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B31" t="s">
         <v>108</v>
@@ -1934,7 +1934,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B32" t="s">
         <v>105</v>
@@ -1942,7 +1942,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B33" t="s">
         <v>109</v>
@@ -1950,7 +1950,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B34" t="s">
         <v>110</v>
@@ -1965,14 +1965,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="71.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
     <col min="6" max="6" width="142.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1998,10 +1999,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
@@ -2015,10 +2016,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
@@ -2027,7 +2028,7 @@
         <v>2020</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -2075,114 +2076,114 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="128" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -2207,16 +2208,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>
@@ -2225,121 +2226,121 @@
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>175</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="C4" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>182</v>
-      </c>
       <c r="D6" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="C7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="C8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
   </sheetData>
@@ -2396,99 +2397,99 @@
         <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>133</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="C2" t="s">
         <v>94</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C3" t="s">
         <v>94</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C4" t="s">
         <v>94</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E4" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E5" t="s">
         <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update CV and Resume
</commit_message>
<xml_diff>
--- a/data/cv.xlsx
+++ b/data/cv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelsieler/Dropbox/Mac (2)/Documents/Project_Repos/curriculum-vitae/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B337126-FD53-8A44-AF78-8FDFE67B0927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C1691-3512-D246-8F91-378CEC16D789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="34560" windowHeight="19800" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="contact" sheetId="1" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="226">
   <si>
     <t>position</t>
   </si>
@@ -84,12 +84,6 @@
     <t>what</t>
   </si>
   <si>
-    <t>HTML</t>
-  </si>
-  <si>
-    <t>Python</t>
-  </si>
-  <si>
     <t>SQL</t>
   </si>
   <si>
@@ -306,12 +300,6 @@
     <t>Git</t>
   </si>
   <si>
-    <t>CSS</t>
-  </si>
-  <si>
-    <t>Markdown</t>
-  </si>
-  <si>
     <t>bash/shell</t>
   </si>
   <si>
@@ -354,15 +342,9 @@
     <t>sielerjm</t>
   </si>
   <si>
-    <t>LaTeX</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
-    <t>C#/Unity</t>
-  </si>
-  <si>
     <t>C++</t>
   </si>
   <si>
@@ -375,52 +357,16 @@
     <t>Microsoft Office Suite</t>
   </si>
   <si>
-    <t>Adobe Photoshop and Illustrator</t>
-  </si>
-  <si>
-    <t>Blender</t>
-  </si>
-  <si>
     <t>German (C1)</t>
   </si>
   <si>
     <t>Spanish (A2)</t>
   </si>
   <si>
-    <t>zebrafish husbandry</t>
-  </si>
-  <si>
-    <t>Bacterial culturing</t>
-  </si>
-  <si>
-    <t>DNA extraction</t>
-  </si>
-  <si>
-    <t>PCR amplification</t>
-  </si>
-  <si>
-    <t>Gel electrophoresis</t>
-  </si>
-  <si>
     <t>16S sequencing</t>
   </si>
   <si>
     <t>Metagenomics</t>
-  </si>
-  <si>
-    <t>DADA2</t>
-  </si>
-  <si>
-    <t>Phyloseq</t>
-  </si>
-  <si>
-    <t>Mothur</t>
-  </si>
-  <si>
-    <t>HMMER</t>
-  </si>
-  <si>
-    <t>FastTree</t>
   </si>
   <si>
     <t>Machine learning</t>
@@ -473,9 +419,6 @@
     <t>projects</t>
   </si>
   <si>
-    <t>[Virtual Fish](https://github.com/OSU-Edu-Games/Virtual-Fish).</t>
-  </si>
-  <si>
     <t>MJSieler Consulting</t>
   </si>
   <si>
@@ -488,9 +431,6 @@
     <t>project</t>
   </si>
   <si>
-    <t>Designed and implemented novel gnotobiotic procedures to process 1,000+ zebrafish embryos to analyze their microbiomes</t>
-  </si>
-  <si>
     <t>Discovering novel antibiotics</t>
   </si>
   <si>
@@ -501,9 +441,6 @@
   </si>
   <si>
     <t>[Virtual Fish](https://github.com/OSU-Edu-Games/Virtual-Fish)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>I'm currently a third year microbiology Ph.D. student minoring in Biological Data Science in the Sharpton Lab at Oregon State University (OSU).</t>
@@ -571,31 +508,16 @@
     <t>Measure resilience of gut microbiome to chronic exposure of antibiotics</t>
   </si>
   <si>
-    <t>Exposed 140 adult zebrafish to varying combinations of antibiotics and controls</t>
-  </si>
-  <si>
     <t>Assess gut microbiome resiliency to anthropological impacts such as temperature and pathogenic exposure</t>
   </si>
   <si>
-    <t>Exposed adult zebrafish to varying combinations of antibiotics and controls</t>
-  </si>
-  <si>
     <t>Investigate the joint interaction effects of pathogen exposure and diet on gut microbiome succession</t>
   </si>
   <si>
-    <t>Fed 180 zebrafish one of three commonly used laboratory diets and exposed half to a common pathogen</t>
-  </si>
-  <si>
     <t>Measure the effect of nanoplastics on the mouse gut microbial community</t>
   </si>
   <si>
-    <t>Statistically analyzed nanoplastic exposure on mouse gut microbial communities</t>
-  </si>
-  <si>
     <t>Meta-analysis of zebrafish gut microbiomes phylogeny</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identified relevant studies and datasets to include in meta-analysis </t>
   </si>
   <si>
     <t>Built and maintain Microbial Bioinformatics Hub to collaboratively share microbiome bioinformatic resources</t>
@@ -629,20 +551,10 @@
     <t>Summary</t>
   </si>
   <si>
-    <t>• Microbiome scientist with 5+ years of experience developing molecular, computational, and statistical research methods
-• Research how multiple environmental factors interact with the gut microbiome to influence host health
-• Robust data analytic skills in multivariate statistics and machine learning to drive research experiments forward
-• Demonstrated abilities to collaborate and take leadership in cross-laboratory experiments
-• Experienced in written, oral and visual communication across scientific and public audiences</t>
-  </si>
-  <si>
     <t>Impacts of diet &amp; infection, temperature &amp; infection, and chronic antibiotic exposure on gut microbiome</t>
   </si>
   <si>
     <t>Designed, developed, and deployed educational video game software for clients to fulfill grant requirements for communicating scientific research.</t>
-  </si>
-  <si>
-    <t>Developed novel gnotobiotic microbiome methods using zebrafish.</t>
   </si>
   <si>
     <t>Assist PhD students and Post-docs with research projects.</t>
@@ -729,24 +641,12 @@
     <t>https://microbial-bioinformatics-hub.readthedocs.io/en/latest/index.html</t>
   </si>
   <si>
-    <t xml:space="preserve">Bacterial culturing, DNA extraction, PCR, Gel Electrophoresis, </t>
-  </si>
-  <si>
-    <t>R, DADA2, Phyloseq, Zebrafish husbandry</t>
-  </si>
-  <si>
-    <t>R, Python, DADA2, Phyloseq, multivariant statistics, machine learning, Unix/Linux, zebrafish husbandry</t>
-  </si>
-  <si>
     <t>C#, Unity, Python, SQL</t>
   </si>
   <si>
     <t>MicrobialBioinformaticsHub</t>
   </si>
   <si>
-    <t>Impacts of diet &amp; infection, temperature &amp; infection, and chronic antibiotic exposure on gut microbiome. [MicrobialBioinformaticsHub](https://microbial-bioinformatics-hub.readthedocs.io/en/latest/index.html)</t>
-  </si>
-  <si>
     <t>https://michaelsieler.com/en/latest/Publications/publications.html</t>
   </si>
   <si>
@@ -754,6 +654,102 @@
   </si>
   <si>
     <t>estimated 2025</t>
+  </si>
+  <si>
+    <t>Impacts of diet &amp; infection, temperature &amp; infection, and chronic antibiotic exposure on gut microbiome. [Microbial Bioinformatics Hub](https://microbial-bioinformatics-hub.readthedocs.io/en/latest/index.html)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://michaelsieler.com/en/latest/Publications/publications.html</t>
+  </si>
+  <si>
+    <t>Zebrafish husbandry</t>
+  </si>
+  <si>
+    <t>Adobe Suite</t>
+  </si>
+  <si>
+    <t>Bacterial culturing, extraction and amplification</t>
+  </si>
+  <si>
+    <t>Transcriptomics</t>
+  </si>
+  <si>
+    <t>Hypothesis testing</t>
+  </si>
+  <si>
+    <t>Big data querying</t>
+  </si>
+  <si>
+    <t>C# (Unity)</t>
+  </si>
+  <si>
+    <t>HTML/CSS</t>
+  </si>
+  <si>
+    <t>Markdown/LaTeX</t>
+  </si>
+  <si>
+    <t>R, Python, Microbial bioinformatics, multivariant statistics, machine learning, Unix/Linux, zebrafish husbandry</t>
+  </si>
+  <si>
+    <t>Sharpton Lab
+(Oregon State University)</t>
+  </si>
+  <si>
+    <t>Sharpton &amp; Mahmud Labs 
+(Oregon State University)</t>
+  </si>
+  <si>
+    <t>R, Microbial bioinformatics, Zebrafish husbandry, molecular wet lab techniques</t>
+  </si>
+  <si>
+    <t>Python (OOP, Numpy,  SciKit, TensorFlow)</t>
+  </si>
+  <si>
+    <t>Developed novel gnotobiotic microbiome methods using 1,500+ zebrafish to assess the impact of environmental toxicants on their gut microbiomes and neurophysiological health.</t>
+  </si>
+  <si>
+    <t>• Designed, developed, and deployed educational video game software for clients to fulfill grant requirements for communicating scientific research</t>
+  </si>
+  <si>
+    <t>Developed novel, high-throughput gnotobiotic microbiome methods to simultaneously process +1000 zebrafish embryos for microbiome and toxicological research</t>
+  </si>
+  <si>
+    <t>Co-authored a paper and contributed a statistical, microbiome analysis on nanoplastic exposure impact on mouse gut microbial communities</t>
+  </si>
+  <si>
+    <t>Co-authored a meta-analysis on environmental exposure impact on zebrafish gut microbiome. Identified, collated, and processed 1000's of 16S sequences from 8 studies for the meta-analysis.</t>
+  </si>
+  <si>
+    <t>Exposed 100+ adult zebrafish to varying combinations of antibiotics to assess chronic antibiotic exposure on the gut microbiomes of zebrafish</t>
+  </si>
+  <si>
+    <t>Exposed 100+ zebrafish to extreme temperatures and parasite exposure to assess anthropological impacts of climage change to the gut microbiomes of zebrafish</t>
+  </si>
+  <si>
+    <t>Administered 100+ zebrafish one of three commonly used laboratory diets and exposed half to a common pathogen to assess diet-pathogen effect on gut microbiome</t>
+  </si>
+  <si>
+    <t>Sieler (in-prep)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Investigate how environmental factors (diet, pollutants, pathogens, etc.) interact with the gut microbiome to influence host health using the zebrafish model organism
+• Developed multivariate statistical and bioinformatic pipelines for analyzing 100's of microbiome samples using R, Python and Command Line Tools
+• Led cross-laboratory scientific experiments from planning, design, implementation and analysis stages using 100's of zebrafish across an array of treatments
+• Co-authored 3 scientific articles
+• Co-taught 70+ student microbiology labs  
+</t>
+  </si>
+  <si>
+    <t>• Developed and implemented novel, high-throughput gnotobiotic microbiome methods to simultaneously process +1000 zebrafish embryos for microbiome and toxicological research
+• Identified dozens of putative antibiotic compound from streptomyces bacteria</t>
+  </si>
+  <si>
+    <t>• Microbiome scientist with 5+ years of experience developing and applying high-throughput molecular, computational, and statistical research methods to analyze 1000's of zebrafish gut microbiome samples
+• Research how multiple environmental factors interact with the gut microbiome to influence host health
+• Robust data analytic skills in multivariate statistics and machine learning propel research experiments forward and gain data-driven insights 
+• Demonstrated abilities to collaborate and take leadership in cross-laboratory experiments and extra-curricular projects
+• Experienced in written, oral and visual communication across scientific and public audiences</t>
   </si>
 </sst>
 </file>
@@ -811,7 +807,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -822,9 +818,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
@@ -1143,10 +1136,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>4</v>
@@ -1157,28 +1150,28 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" t="s">
+        <v>90</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B2" t="s">
+      <c r="F2" t="s">
         <v>93</v>
       </c>
-      <c r="C2" t="s">
+      <c r="G2" t="s">
         <v>94</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="H2" t="s">
         <v>95</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="F2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G2" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" t="s">
-        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1206,7 +1199,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1215,31 +1208,31 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>198</v>
+        <v>170</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>169</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" s="4">
         <v>2020</v>
@@ -1248,40 +1241,40 @@
         <v>2023</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>203</v>
+        <v>175</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>205</v>
+        <v>177</v>
       </c>
       <c r="H2" s="7" t="s">
-        <v>204</v>
+        <v>176</v>
       </c>
       <c r="I2" s="4"/>
     </row>
     <row r="3" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>171</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>200</v>
+        <v>172</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>173</v>
       </c>
       <c r="D3">
         <v>2020</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>202</v>
+        <v>174</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>207</v>
+        <v>179</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>206</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1313,43 +1306,43 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G1" s="4"/>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>209</v>
+        <v>181</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>208</v>
+        <v>180</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>212</v>
+        <v>184</v>
       </c>
       <c r="D2">
         <v>2021</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>211</v>
+        <v>183</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>210</v>
+        <v>182</v>
       </c>
       <c r="G2" s="4"/>
     </row>
@@ -1381,62 +1374,62 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>159</v>
+        <v>138</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>155</v>
+        <v>134</v>
       </c>
       <c r="D2">
         <v>2022</v>
       </c>
       <c r="E2" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>164</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="D3">
         <v>2021</v>
       </c>
       <c r="E3" t="s">
-        <v>166</v>
+        <v>145</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>165</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1457,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -1470,30 +1463,30 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="D2">
         <v>2019</v>
@@ -1501,13 +1494,13 @@
     </row>
     <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>161</v>
+        <v>140</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <v>2019</v>
@@ -1529,7 +1522,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1540,23 +1533,24 @@
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>228</v>
+        <v>195</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{3AAB4D94-B1E8-964F-9129-1CDB5078C887}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{3DC17D74-10AD-EA4C-A5CB-8763C5723CA4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1567,7 +1561,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1579,27 +1573,27 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="224" x14ac:dyDescent="0.2">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="240" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -1607,13 +1601,13 @@
     </row>
     <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -1621,13 +1615,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -1635,13 +1629,13 @@
     </row>
     <row r="5" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -1649,13 +1643,13 @@
     </row>
     <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -1663,13 +1657,13 @@
     </row>
     <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B7">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -1682,16 +1676,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1704,266 +1698,202 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B9" t="s">
-        <v>84</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>163</v>
+        <v>142</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
       <c r="B12" t="s">
-        <v>100</v>
+        <v>205</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B13" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B17" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>118</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>127</v>
+        <v>141</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>202</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
+      </c>
+      <c r="B22" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B23" t="s">
-        <v>122</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>111</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>162</v>
-      </c>
-      <c r="B27" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>128</v>
-      </c>
-      <c r="B30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>129</v>
-      </c>
-      <c r="B32" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>129</v>
-      </c>
-      <c r="B34" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1989,33 +1919,33 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2">
         <v>2017</v>
@@ -2026,19 +1956,19 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="B3" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3">
         <v>2020</v>
       </c>
       <c r="E3" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2048,10 +1978,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F82E9F-5F43-C245-8CAF-20E15947BB6A}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2077,123 +2007,97 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>134</v>
+        <v>211</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>90</v>
+      </c>
+      <c r="D2" t="s">
+        <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>194</v>
+        <v>224</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="176" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
-      </c>
-      <c r="D3" t="s">
-        <v>168</v>
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>146</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>193</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="128" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>131</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -2205,8 +2109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94F99B80-F261-274F-ACFD-5BA2CCD61FB4}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2218,139 +2122,139 @@
   <sheetData>
     <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>143</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>213</v>
+        <v>185</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="112" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>174</v>
+        <v>151</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>175</v>
+        <v>221</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>217</v>
+        <v>222</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="96" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>170</v>
-      </c>
       <c r="B4" s="1" t="s">
-        <v>171</v>
+        <v>219</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>217</v>
+        <v>189</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="96" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>142</v>
+        <v>123</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>144</v>
+        <v>216</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>216</v>
+        <v>188</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="128" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>225</v>
+        <v>194</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>220</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>179</v>
+        <v>218</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>214</v>
+        <v>186</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>215</v>
+        <v>187</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -2372,7 +2276,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="C2:E5"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2398,108 +2302,108 @@
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>18</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C2" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>169</v>
+        <v>148</v>
       </c>
       <c r="E2" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>194</v>
+        <v>166</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>145</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>168</v>
+        <v>147</v>
       </c>
       <c r="E3" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>193</v>
+        <v>214</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>146</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="64" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>167</v>
+        <v>146</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>147</v>
+        <v>127</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>191</v>
+        <v>164</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>192</v>
+        <v>165</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2526,138 +2430,138 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2686,163 +2590,163 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" t="s">
-        <v>45</v>
-      </c>
       <c r="D2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
         <v>39</v>
       </c>
-      <c r="B3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
       <c r="D3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" t="s">
         <v>35</v>
-      </c>
-      <c r="C4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E4" t="s">
-        <v>37</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" t="s">
         <v>56</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>37</v>
-      </c>
-      <c r="F5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C6" t="s">
         <v>63</v>
       </c>
-      <c r="B6" t="s">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
       <c r="D6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>